<commit_message>
feat: add form components with react-hook-form integration and select component implementation
- Introduced a new Form component with FormField, FormItem, FormLabel, FormControl, FormDescription, and FormMessage for better form handling using react-hook-form.
- Implemented context for form fields to manage state and validation messages.
- Created a Select component with various subcomponents including SelectTrigger, SelectContent, SelectItem, SelectLabel, and scroll buttons for enhanced dropdown functionality.
- Utilized Radix UI primitives for building accessible and customizable form and select components.
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -1,29 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_StudyDocument\Cybersoft\project_airbnb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_StudyDocument\Cybersoft\FE\project_airbnb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCFC100-009E-4FB6-B4C6-EC37471C7944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BCF20F-1486-4A34-B6F7-A7336347642B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>Thêm, xoá, sửa phòng đã đặt</t>
+  </si>
+  <si>
+    <t>13/09</t>
   </si>
 </sst>
 </file>
@@ -347,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -409,6 +409,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -655,7 +658,7 @@
   <dimension ref="A1:J1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -789,9 +792,15 @@
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
+      <c r="B8" s="8">
+        <v>45756</v>
+      </c>
+      <c r="C8" s="8">
+        <v>45756</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
       <c r="E8" s="10" t="s">
         <v>9</v>
       </c>
@@ -805,9 +814,15 @@
       <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
+      <c r="B9" s="8">
+        <v>45786</v>
+      </c>
+      <c r="C9" s="8">
+        <v>45786</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
       <c r="E9" s="10" t="s">
         <v>9</v>
       </c>
@@ -821,9 +836,15 @@
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="8">
+        <v>45786</v>
+      </c>
+      <c r="C10" s="8">
+        <v>45786</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
       <c r="E10" s="10" t="s">
         <v>9</v>
       </c>
@@ -837,9 +858,15 @@
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
+      <c r="B11" s="8">
+        <v>45817</v>
+      </c>
+      <c r="C11" s="8">
+        <v>45817</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
       <c r="E11" s="10" t="s">
         <v>9</v>
       </c>
@@ -853,9 +880,15 @@
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
+      <c r="B12" s="8">
+        <v>45847</v>
+      </c>
+      <c r="C12" s="8">
+        <v>45847</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
       <c r="E12" s="10" t="s">
         <v>9</v>
       </c>
@@ -869,9 +902,15 @@
       <c r="A13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="8">
+        <v>45878</v>
+      </c>
+      <c r="C13" s="8">
+        <v>45878</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
       <c r="E13" s="10" t="s">
         <v>9</v>
       </c>
@@ -885,9 +924,15 @@
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
+      <c r="B14" s="8">
+        <v>45909</v>
+      </c>
+      <c r="C14" s="8">
+        <v>45939</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
       <c r="E14" s="10" t="s">
         <v>9</v>
       </c>
@@ -901,9 +946,15 @@
       <c r="A15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
+      <c r="B15" s="8">
+        <v>45970</v>
+      </c>
+      <c r="C15" s="8">
+        <v>46000</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
       <c r="E15" s="10" t="s">
         <v>9</v>
       </c>
@@ -917,9 +968,15 @@
       <c r="A16" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
+      <c r="B16" s="8">
+        <v>45970</v>
+      </c>
+      <c r="C16" s="8">
+        <v>46000</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
       <c r="E16" s="10" t="s">
         <v>9</v>
       </c>
@@ -933,9 +990,15 @@
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
+      <c r="B17" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
       <c r="E17" s="10" t="s">
         <v>9</v>
       </c>
@@ -949,9 +1012,15 @@
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
+      <c r="B18" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
       <c r="E18" s="10" t="s">
         <v>9</v>
       </c>
@@ -969,7 +1038,7 @@
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -985,7 +1054,7 @@
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
       <c r="E20" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
@@ -1001,7 +1070,7 @@
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
@@ -1097,7 +1166,7 @@
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="20" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -1113,7 +1182,7 @@
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
       <c r="E28" s="20" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>

</xml_diff>